<commit_message>
Updated Status. Added layout to action items.
</commit_message>
<xml_diff>
--- a/Project Details/Action Items.xlsx
+++ b/Project Details/Action Items.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ACTION ITEMS</t>
   </si>
@@ -72,13 +72,25 @@
     <t xml:space="preserve"> Use board rules from OSH Park.com</t>
   </si>
   <si>
-    <t>Include all that it would take to make one board</t>
-  </si>
-  <si>
     <t>Research onboard programming</t>
   </si>
   <si>
     <t>Probably SPI</t>
+  </si>
+  <si>
+    <t>Include all that it would take to make 6 units.</t>
+  </si>
+  <si>
+    <t>BUILD</t>
+  </si>
+  <si>
+    <t>UNIT LAYOUT</t>
+  </si>
+  <si>
+    <t>HOUSING</t>
+  </si>
+  <si>
+    <t>PREMADE OR ACRYLIC</t>
   </si>
 </sst>
 </file>
@@ -138,14 +150,14 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,7 +463,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,254 +489,266 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3">
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.1</v>
-      </c>
-    </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Added part verification needed for schematic.
</commit_message>
<xml_diff>
--- a/Project Details/Action Items.xlsx
+++ b/Project Details/Action Items.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ACTION ITEMS</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>PREMADE OR ACRYLIC</t>
+  </si>
+  <si>
+    <t>Part Verification</t>
+  </si>
+  <si>
+    <t>Size, Value, Make, Female</t>
   </si>
 </sst>
 </file>
@@ -462,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,12 +638,18 @@
       <c r="C18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>